<commit_message>
added sphinx to do documentation, debugged a bit
</commit_message>
<xml_diff>
--- a/DATA/inputs.xlsx
+++ b/DATA/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maceo.valente\Documents\Automatisation\TEST_MVA\TSAgriPV\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA0678F-A9E4-47DA-9760-EA5701A68915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BB215E-5231-43D9-821D-B99DF65B9713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="148">
   <si>
     <t>Entraxe</t>
   </si>
@@ -161,9 +161,6 @@
     <t>PY_FINESSE</t>
   </si>
   <si>
-    <t>PY_cepage</t>
-  </si>
-  <si>
     <t>[0,0,0,0,0]</t>
   </si>
   <si>
@@ -363,9 +360,6 @@
   </si>
   <si>
     <t>[-90 ; 0] °, Angle de début de course autour de l'axe N-S</t>
-  </si>
-  <si>
-    <t>[0 ; 90] °, Angle de début de course autour de l'axe N-S</t>
   </si>
   <si>
     <t>Nom EPW</t>
@@ -535,6 +529,27 @@
   </si>
   <si>
     <t>garcia</t>
+  </si>
+  <si>
+    <t>[0 ; 90] °, Angle de fin de course autour de l'axe N-S</t>
+  </si>
+  <si>
+    <t>TECPL_codecalirrig</t>
+  </si>
+  <si>
+    <t>Irrigation</t>
+  </si>
+  <si>
+    <t>[1 ou 2] Activation de l'irrigation (1) ou non (2). Irrigation activée = param swfac supérieur à 0.45</t>
+  </si>
+  <si>
+    <t>Fichier plante, à modifier parmi la liste de fichiers plantes, visible sur STICS, global parameters, plant and genotype</t>
+  </si>
+  <si>
+    <t>USMSS_fplt</t>
+  </si>
+  <si>
+    <t>vine_PINCC_plt.xml</t>
   </si>
 </sst>
 </file>
@@ -859,18 +874,20 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -894,24 +911,29 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -922,8 +944,56 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -934,77 +1004,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1286,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,71 +1327,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="52" t="s">
+      <c r="A1" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="48"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="36"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -1386,10 +1409,10 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -1407,10 +1430,10 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -1431,19 +1454,19 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50"/>
+      <c r="K6" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -1455,21 +1478,21 @@
       <c r="C7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="32"/>
+      <c r="D7" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="24"/>
       <c r="O7" s="8">
         <v>2.25</v>
       </c>
@@ -1488,19 +1511,19 @@
       <c r="C8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="32"/>
+      <c r="D8" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="8">
         <v>6</v>
       </c>
@@ -1519,19 +1542,19 @@
       <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="32"/>
+      <c r="D9" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="24"/>
       <c r="O9" s="8">
         <v>1.135</v>
       </c>
@@ -1550,19 +1573,19 @@
       <c r="C10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="32"/>
+      <c r="D10" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="24"/>
       <c r="O10" s="8">
         <v>0</v>
       </c>
@@ -1573,27 +1596,27 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B11" s="5">
         <v>50</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="32"/>
+        <v>117</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="14">
         <v>50</v>
       </c>
@@ -1604,27 +1627,27 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B12" s="5">
         <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="32"/>
+        <v>118</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="14">
         <v>10</v>
       </c>
@@ -1643,19 +1666,19 @@
       <c r="C13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="32"/>
+      <c r="D13" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="24"/>
       <c r="O13" s="8">
         <v>0.18</v>
       </c>
@@ -1674,19 +1697,19 @@
       <c r="C14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="32"/>
+      <c r="D14" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="24"/>
       <c r="O14" s="8">
         <v>4</v>
       </c>
@@ -1705,19 +1728,19 @@
       <c r="C15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="32"/>
+      <c r="D15" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="24"/>
       <c r="O15" s="8">
         <v>13</v>
       </c>
@@ -1728,27 +1751,27 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="5">
         <v>-60</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="32"/>
+        <v>103</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="24"/>
       <c r="O16" s="14">
         <v>-60</v>
       </c>
@@ -1759,27 +1782,27 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="5">
         <v>60</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="32"/>
+        <v>104</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="24"/>
       <c r="O17" s="14">
         <v>60</v>
       </c>
@@ -1790,27 +1813,27 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="5">
         <v>60</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="32"/>
+        <v>73</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="24"/>
       <c r="O18" s="14">
         <v>60</v>
       </c>
@@ -1821,29 +1844,29 @@
     </row>
     <row r="19" spans="1:19" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B19" s="16">
         <v>0</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="32"/>
+        <v>132</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="24"/>
       <c r="O19" s="14">
         <v>1</v>
       </c>
@@ -1862,19 +1885,19 @@
       <c r="C20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="32"/>
+      <c r="D20" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="24"/>
       <c r="O20" s="8">
         <v>1</v>
       </c>
@@ -1893,19 +1916,19 @@
       <c r="C21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="32"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="24"/>
       <c r="O21" s="8">
         <v>1</v>
       </c>
@@ -1916,27 +1939,27 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="32"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="24"/>
       <c r="O22" s="8">
         <v>10000</v>
       </c>
@@ -1947,29 +1970,29 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="32"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="24"/>
       <c r="O23" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -1978,29 +2001,29 @@
     </row>
     <row r="24" spans="1:19" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="32"/>
+        <v>128</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="24"/>
       <c r="O24" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -2009,27 +2032,27 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="32"/>
+        <v>113</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="24"/>
       <c r="O25" s="14">
         <v>1</v>
       </c>
@@ -2040,7 +2063,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" s="5">
         <v>35.799999999999997</v>
@@ -2048,21 +2071,21 @@
       <c r="C26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="29"/>
+      <c r="D26" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="46"/>
       <c r="O26" s="10">
         <v>35.799999999999997</v>
       </c>
@@ -2073,7 +2096,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="5">
         <v>0.15</v>
@@ -2081,19 +2104,19 @@
       <c r="C27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="29"/>
+      <c r="D27" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="46"/>
       <c r="O27" s="10">
         <v>0.15</v>
       </c>
@@ -2104,7 +2127,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="5">
         <v>22</v>
@@ -2112,19 +2135,19 @@
       <c r="C28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="29"/>
+      <c r="D28" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="46"/>
       <c r="O28" s="10">
         <v>22</v>
       </c>
@@ -2135,7 +2158,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="5">
         <v>35</v>
@@ -2144,7 +2167,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2152,10 +2175,10 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="11"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="29"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="46"/>
       <c r="O29" s="10">
         <v>35</v>
       </c>
@@ -2166,7 +2189,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="5">
         <v>10</v>
@@ -2174,19 +2197,19 @@
       <c r="C30" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="29"/>
+      <c r="D30" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="46"/>
       <c r="O30" s="10">
         <v>10</v>
       </c>
@@ -2197,7 +2220,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="5">
         <v>8.1999999999999993</v>
@@ -2205,19 +2228,19 @@
       <c r="C31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="29"/>
+      <c r="D31" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="46"/>
       <c r="O31" s="10">
         <v>8.1999999999999993</v>
       </c>
@@ -2228,7 +2251,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>16</v>
@@ -2236,19 +2259,19 @@
       <c r="C32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="29"/>
+      <c r="D32" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="46"/>
       <c r="O32" s="10" t="s">
         <v>16</v>
       </c>
@@ -2259,29 +2282,29 @@
     </row>
     <row r="33" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="29"/>
+      <c r="D33" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="46"/>
       <c r="O33" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
@@ -2290,27 +2313,27 @@
     </row>
     <row r="34" spans="1:19" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="29"/>
+        <v>76</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="46"/>
       <c r="O34" s="10" t="s">
         <v>25</v>
       </c>
@@ -2321,7 +2344,7 @@
     </row>
     <row r="35" spans="1:19" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>26</v>
@@ -2329,19 +2352,19 @@
       <c r="C35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="28"/>
-      <c r="N35" s="29"/>
+      <c r="D35" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="46"/>
       <c r="O35" s="10" t="s">
         <v>26</v>
       </c>
@@ -2352,7 +2375,7 @@
     </row>
     <row r="36" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>28</v>
@@ -2360,19 +2383,19 @@
       <c r="C36" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
-      <c r="N36" s="29"/>
+      <c r="D36" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="46"/>
       <c r="O36" s="10" t="s">
         <v>28</v>
       </c>
@@ -2383,29 +2406,29 @@
     </row>
     <row r="37" spans="1:19" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="29"/>
+      <c r="D37" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="46"/>
       <c r="O37" s="10" t="s">
         <v>30</v>
       </c>
@@ -2416,29 +2439,29 @@
     </row>
     <row r="38" spans="1:19" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="29"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="46"/>
       <c r="O38" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
@@ -2447,29 +2470,29 @@
     </row>
     <row r="39" spans="1:19" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="29"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="46"/>
       <c r="O39" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
@@ -2478,29 +2501,29 @@
     </row>
     <row r="40" spans="1:19" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="29"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="46"/>
       <c r="O40" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
@@ -2509,29 +2532,29 @@
     </row>
     <row r="41" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" s="5">
         <v>213</v>
       </c>
       <c r="C41" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="29"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="24"/>
       <c r="O41" s="10">
         <v>213</v>
       </c>
@@ -2542,27 +2565,27 @@
     </row>
     <row r="42" spans="1:19" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" s="5">
         <v>730</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="29"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="24"/>
       <c r="O42" s="10">
         <v>730</v>
       </c>
@@ -2571,33 +2594,31 @@
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="5">
-        <v>5</v>
+    <row r="43" spans="1:19" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="52" t="s">
+        <v>147</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="10">
-        <v>5</v>
+        <v>146</v>
+      </c>
+      <c r="D43" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="54"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="56"/>
+      <c r="O43" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
@@ -2606,29 +2627,31 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B44" s="5">
-        <v>0.44</v>
+        <v>5</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="29"/>
+        <v>68</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="24"/>
       <c r="O44" s="10">
-        <v>0.44</v>
+        <v>5</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -2636,61 +2659,91 @@
       <c r="S44" s="2"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>15</v>
+      <c r="A45" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0.44</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="10" t="s">
-        <v>15</v>
+        <v>71</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="10">
+        <v>0.44</v>
       </c>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
+    <row r="46" spans="1:19" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="5">
+        <v>2</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="10">
+        <v>1</v>
+      </c>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="A1:N3"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="P1:S5"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K7:N18"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="K41:N43"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="K44:N46"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="K26:N36"/>
+    <mergeCell ref="K37:N40"/>
+    <mergeCell ref="K19:N25"/>
+    <mergeCell ref="D45:J45"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="D41:J41"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="D44:J44"/>
     <mergeCell ref="D38:J38"/>
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="D26:J26"/>
@@ -2707,22 +2760,24 @@
     <mergeCell ref="D37:J37"/>
     <mergeCell ref="D24:J24"/>
     <mergeCell ref="D22:J22"/>
-    <mergeCell ref="D45:J45"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="D23:J23"/>
-    <mergeCell ref="K26:N36"/>
-    <mergeCell ref="K37:N40"/>
-    <mergeCell ref="K41:N42"/>
-    <mergeCell ref="K43:N44"/>
-    <mergeCell ref="K19:N25"/>
-    <mergeCell ref="D44:J44"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="D41:J41"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="A1:N3"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="P1:S5"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K7:N18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>